<commit_message>
Experiment 2: add PCIbex scripts
</commit_message>
<xml_diff>
--- a/materials/characters.xlsx
+++ b/materials/characters.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\betha\Google Drive\Lab\Singular They Memory\singular-they-memory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\betha\My Drive\Project_They\Singular-They-Public\materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0301938-4A57-4E62-8023-8979C5E4AA37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0163D98-9581-4D19-87EB-F77A7946D2BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="804" windowWidth="10188" windowHeight="11556" activeTab="1" xr2:uid="{31D6D30D-2501-4341-A423-AA8567237050}"/>
+    <workbookView xWindow="1740" yWindow="3432" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{31D6D30D-2501-4341-A423-AA8567237050}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
     <sheet name="Lists" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -325,14 +325,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,9 +651,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="10.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -675,130 +670,130 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C5" s="2" t="s">
+      <c r="C5" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C8" s="2" t="s">
+      <c r="C8" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C9" s="2" t="s">
+      <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C12" s="2" t="s">
+      <c r="C12" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C13" s="2" t="s">
+      <c r="C13" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+      <c r="A14">
         <v>3</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14">
         <v>3</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14">
         <v>12</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14">
         <v>12</v>
       </c>
     </row>
@@ -810,27 +805,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08FF7647-0A2D-4CF1-9C22-E2549270EF8E}">
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L44" sqref="L44"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="119" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="4" customWidth="1"/>
-    <col min="6" max="14" width="10.6640625" customWidth="1"/>
+    <col min="1" max="14" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -845,245 +838,234 @@
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="2"/>
       <c r="L2" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="2"/>
       <c r="L3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="2"/>
       <c r="L7" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="2"/>
       <c r="L11" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="A14" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
@@ -1098,41 +1080,41 @@
       <c r="D17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" t="s">
         <v>55</v>
       </c>
       <c r="L19" t="s">
@@ -1140,104 +1122,104 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="A23" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="A24" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="A25" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" t="s">
         <v>61</v>
       </c>
       <c r="L25" t="s">
@@ -1245,19 +1227,19 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="A26" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E26" t="s">
         <v>62</v>
       </c>
       <c r="L26" t="s">
@@ -1265,67 +1247,64 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="A27" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="A28" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" t="s">
         <v>17</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E28" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+      <c r="A29" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E29" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="2"/>
-    </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
@@ -1340,75 +1319,75 @@
       <c r="D32" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
+      <c r="A33" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" t="s">
         <v>25</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="E33" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+      <c r="A34" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" t="s">
         <v>15</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+      <c r="A35" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" t="s">
         <v>17</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="E35" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
+      <c r="A36" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" t="s">
         <v>29</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" t="s">
         <v>20</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E36" t="s">
         <v>69</v>
       </c>
       <c r="L36" t="s">
@@ -1416,53 +1395,53 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
+      <c r="A37" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" t="s">
         <v>19</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="E37" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
+      <c r="A38" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" t="s">
         <v>22</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" t="s">
         <v>7</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" t="s">
         <v>11</v>
       </c>
-      <c r="E38" s="6" t="s">
+      <c r="E38" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
+      <c r="A39" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" t="s">
         <v>25</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="E39" t="s">
         <v>72</v>
       </c>
       <c r="L39" t="s">
@@ -1470,87 +1449,87 @@
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
+      <c r="A40" t="s">
         <v>2</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" t="s">
         <v>31</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" t="s">
         <v>6</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" t="s">
         <v>12</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="E40" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
+      <c r="A41" t="s">
         <v>3</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" t="s">
         <v>7</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" t="s">
         <v>9</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="E41" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
+      <c r="A42" t="s">
         <v>3</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" t="s">
         <v>23</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" t="s">
         <v>25</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" t="s">
         <v>18</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="E42" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
+      <c r="A43" t="s">
         <v>3</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" t="s">
         <v>33</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" t="s">
         <v>6</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" t="s">
         <v>16</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="E43" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
+      <c r="A44" t="s">
         <v>3</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" t="s">
         <v>7</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" t="s">
         <v>13</v>
       </c>
-      <c r="E44" s="6" t="s">
+      <c r="E44" t="s">
         <v>77</v>
       </c>
       <c r="L44" t="s">
@@ -1558,66 +1537,30 @@
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
-      <c r="E47" s="5"/>
+      <c r="E47" s="1"/>
       <c r="F47" s="1"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="6"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="3"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="6"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="6"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="6"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="6"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="6"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>